<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@bc3e57130398985a37185af7a6440121382e4dbf 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-hash-extension.xlsx
+++ b/StructureDefinition-hash-extension.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-21T16:00:02+00:00</t>
+    <t>2025-07-21T16:06:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -306,10 +306,10 @@
     <t>Element.extension</t>
   </si>
   <si>
-    <t>Extension.extension:hash-value</t>
-  </si>
-  <si>
-    <t>hash-value</t>
+    <t>Extension.extension:hashValue</t>
+  </si>
+  <si>
+    <t>hashValue</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {https://nih-ncpi.github.io/ncpi-fhir-ig-2/StructureDefinition/hash-value}
@@ -319,10 +319,10 @@
     <t>Value of hashing the file</t>
   </si>
   <si>
-    <t>Extension.extension:hash-type</t>
-  </si>
-  <si>
-    <t>hash-type</t>
+    <t>Extension.extension:hashType</t>
+  </si>
+  <si>
+    <t>hashType</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {https://nih-ncpi.github.io/ncpi-fhir-ig-2/StructureDefinition/hash-type}
@@ -687,7 +687,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="25.96484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="25.54296875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>